<commit_message>
Matriz de Confusion y VFPN
</commit_message>
<xml_diff>
--- a/MATRIZ Y.xlsx
+++ b/MATRIZ Y.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJ\Documents\poryectoRostro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D338525-2DC5-4169-BFE2-76D86EB8152E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9BE7CA-A0AB-4858-8E49-1E40F23D97E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="492" windowWidth="22692" windowHeight="10380" xr2:uid="{55C39581-0358-4A7E-BE22-F5C43957E6F7}"/>
   </bookViews>
@@ -686,9 +686,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44E9E09-86EA-4A35-A9E1-3E672D085690}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -696,12 +698,12 @@
     <col min="2" max="2" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,8 +711,15 @@
         <f>IF(ISNUMBER(FIND("mujer",A2)),-1,1)</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(B2=C2,"VERDADERO","X")</f>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -718,8 +727,15 @@
         <f t="shared" ref="B3:B66" si="0">IF(ISNUMBER(FIND("mujer",A3)),-1,1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="1">IF(B3=C3,"VERDADERO","X")</f>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -727,8 +743,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -736,8 +759,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -745,8 +775,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -754,8 +791,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -763,8 +807,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -772,8 +823,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -781,8 +839,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -790,8 +855,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -799,8 +871,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -808,8 +887,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -817,8 +903,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -826,8 +919,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -835,8 +935,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -844,8 +951,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -853,8 +967,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -862,8 +983,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -871,8 +999,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -880,8 +1015,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>-1</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -889,8 +1031,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -898,8 +1047,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -907,8 +1063,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>-1</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -916,8 +1079,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -925,8 +1095,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -934,8 +1111,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -943,8 +1127,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -952,8 +1143,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -961,8 +1159,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -970,8 +1175,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>-1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -979,8 +1191,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>-1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -988,8 +1207,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -997,8 +1223,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1006,8 +1239,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1015,8 +1255,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>-1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1024,8 +1271,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>-1</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1033,8 +1287,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>-1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1042,8 +1303,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>-1</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1051,8 +1319,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1060,8 +1335,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1069,8 +1351,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>-1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1078,8 +1367,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>-1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1087,8 +1383,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>-1</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1096,8 +1399,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1105,8 +1415,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1114,8 +1431,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1123,8 +1447,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1132,8 +1463,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>-1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1141,8 +1479,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>-1</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1150,8 +1495,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1159,8 +1511,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1168,8 +1527,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1177,8 +1543,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>-1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1186,8 +1559,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1195,8 +1575,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1204,8 +1591,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>-1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1213,8 +1607,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>-1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1222,8 +1623,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1231,8 +1639,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>-1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1240,8 +1655,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>-1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1249,8 +1671,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>-1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -1258,8 +1687,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1267,8 +1703,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>-1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -1276,8 +1719,15 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>-1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1285,320 +1735,572 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B101" si="1">IF(ISNUMBER(FIND("mujer",A67)),-1,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" ref="B67:B101" si="2">IF(ISNUMBER(FIND("mujer",A67)),-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D101" si="3">IF(B67=C67,"VERDADERO","X")</f>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C68">
+        <v>-1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C71">
+        <v>-1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C72">
+        <v>-1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C73">
+        <v>-1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C74">
+        <v>-1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C80">
+        <v>-1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C81">
+        <v>-1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B82">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B83">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B84">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C84">
+        <v>-1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B85">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C85">
+        <v>-1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B86">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B87">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C87">
+        <v>-1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B88">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B89">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B90">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C90">
+        <v>-1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B91">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B92">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B93">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B94">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C94">
+        <v>-1</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B95">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B96">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C96">
+        <v>-1</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B97">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C97">
+        <v>-1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B98">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C98">
+        <v>-1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B99">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="C99">
+        <v>-1</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B100">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B101">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="3"/>
+        <v>VERDADERO</v>
       </c>
     </row>
   </sheetData>

</xml_diff>